<commit_message>
add full manage dialog functionality
</commit_message>
<xml_diff>
--- a/wdc_libs/data-examples/dataset-example.xlsx
+++ b/wdc_libs/data-examples/dataset-example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="15120" windowHeight="7830" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="15120" windowHeight="7830"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="5" r:id="rId1"/>
@@ -1574,9 +1574,6 @@
     <t>HEAD</t>
   </si>
   <si>
-    <t>dataset.visibility</t>
-  </si>
-  <si>
     <t>public</t>
   </si>
   <si>
@@ -1679,9 +1676,6 @@
     <t>Світові індикатори розвитку/Економіка/ВВП</t>
   </si>
   <si>
-    <t>Andrey Boldak</t>
-  </si>
-  <si>
     <t>#EC</t>
   </si>
   <si>
@@ -1710,6 +1704,12 @@
   </si>
   <si>
     <t>http://www.pnglogo.com/wp-content/uploads/2015/10/Economy-Rise-PNG-02088.png</t>
+  </si>
+  <si>
+    <t>dataset.status</t>
+  </si>
+  <si>
+    <t>Vasya</t>
   </si>
 </sst>
 </file>
@@ -2152,8 +2152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2176,15 +2176,15 @@
         <v>22</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
+        <v>561</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>517</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2197,10 +2197,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>552</v>
+        <v>562</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2213,16 +2213,16 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B7" s="13">
         <f ca="1">TODAY()</f>
-        <v>42339</v>
+        <v>42341</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>516</v>
@@ -2238,18 +2238,18 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2265,15 +2265,15 @@
         <v>35</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2286,10 +2286,10 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2302,10 +2302,10 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2389,7 +2389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -2409,19 +2409,19 @@
         <v>11</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>538</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>539</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>540</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>541</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -2432,10 +2432,10 @@
         <v>23</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>30</v>
@@ -2446,19 +2446,19 @@
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2469,13 +2469,13 @@
         <v>26</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2486,7 +2486,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2540,26 +2540,26 @@
         <v>11</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>542</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>543</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>6</v>
@@ -2570,7 +2570,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>18</v>
@@ -2581,18 +2581,18 @@
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>31</v>
@@ -2603,29 +2603,29 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>525</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>526</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>14</v>
@@ -2636,7 +2636,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>15</v>
@@ -2647,7 +2647,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>9</v>
@@ -2658,35 +2658,35 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
+        <v>548</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>549</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="C12" s="15" t="s">
         <v>550</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
+        <v>552</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>553</v>
+      </c>
+      <c r="C13" s="15" t="s">
         <v>554</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>555</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
+        <v>557</v>
+      </c>
+      <c r="B14" t="s">
         <v>559</v>
       </c>
-      <c r="B14" t="s">
-        <v>561</v>
-      </c>
       <c r="C14" s="16" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add advanced commit's management
</commit_message>
<xml_diff>
--- a/wdc_libs/data-examples/dataset-example.xlsx
+++ b/wdc_libs/data-examples/dataset-example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="15120" windowHeight="7830"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="15120" windowHeight="7830" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="5" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4562" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4573" uniqueCount="572">
   <si>
     <t>Country Name</t>
   </si>
@@ -1710,13 +1710,40 @@
   </si>
   <si>
     <t>Vasya</t>
+  </si>
+  <si>
+    <t>Andrey Boldak</t>
+  </si>
+  <si>
+    <t>#BOLDAK_NAME</t>
+  </si>
+  <si>
+    <t>http://wdc.org.ua/sites/default/files/imagepicker/25/a_boldac.png</t>
+  </si>
+  <si>
+    <t>#BOLDAK_INFO</t>
+  </si>
+  <si>
+    <t>mailto:boldak@wdc.org.ua</t>
+  </si>
+  <si>
+    <t>Andriy Boldak</t>
+  </si>
+  <si>
+    <t>Areas of scientific interests: data reliability, validity and consistency, multivariate data exploration techniques, data integration and indices design, application of cause-effect models, image processing and patterns recognition, design and development information system.</t>
+  </si>
+  <si>
+    <t>Болдак Андрій Олександрович</t>
+  </si>
+  <si>
+    <t>Коло наукових інтересів: надійність, обґрунтованість і послідовність даних, методи дослідження багатовимірних даних, інтеграція даних і проектування показників, застосування причинно-наслідкових моделей, обробка зображень і розпізнавання образів, інформаційна система проектування і розробки.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1756,6 +1783,15 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1765,7 +1801,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1799,12 +1835,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1848,8 +1894,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Гиперссылка" xfId="2" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1"/>
   </cellStyles>
@@ -2152,7 +2205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -2217,7 +2270,7 @@
       </c>
       <c r="B7" s="13">
         <f ca="1">TODAY()</f>
-        <v>42341</v>
+        <v>42342</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2389,8 +2442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2511,22 +2564,42 @@
         <v>48</v>
       </c>
     </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>563</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>564</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>566</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>565</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>567</v>
+      </c>
+    </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="B1:B7"/>
+  <hyperlinks>
+    <hyperlink ref="F8" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2687,6 +2760,28 @@
       </c>
       <c r="C14" s="16" t="s">
         <v>558</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>564</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>568</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>566</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>569</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>571</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add query dialog functionality
</commit_message>
<xml_diff>
--- a/wdc_libs/data-examples/dataset-example.xlsx
+++ b/wdc_libs/data-examples/dataset-example.xlsx
@@ -13,7 +13,7 @@
     <sheet name="data" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">data!$A$1:$F$887</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">data!$A$1:$A$887</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">dictionary!$B$1:$B$7</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4573" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4579" uniqueCount="576">
   <si>
     <t>Country Name</t>
   </si>
@@ -1737,6 +1737,18 @@
   </si>
   <si>
     <t>Коло наукових інтересів: надійність, обґрунтованість і послідовність даних, методи дослідження багатовимірних даних, інтеграція даних і проектування показників, застосування причинно-наслідкових моделей, обробка зображень і розпізнавання образів, інформаційна система проектування і розробки.</t>
+  </si>
+  <si>
+    <t>#UKR</t>
+  </si>
+  <si>
+    <t>#UKR_LABEL</t>
+  </si>
+  <si>
+    <t>Україна</t>
+  </si>
+  <si>
+    <t>https://flagspot.net/images/u/ua.gif</t>
   </si>
 </sst>
 </file>
@@ -1850,7 +1862,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1899,6 +1911,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2270,7 +2289,7 @@
       </c>
       <c r="B7" s="13">
         <f ca="1">TODAY()</f>
-        <v>42342</v>
+        <v>42346</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2442,8 +2461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2581,6 +2600,20 @@
         <v>567</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>572</v>
+      </c>
+      <c r="B9" s="19"/>
+      <c r="C9" s="20" t="s">
+        <v>573</v>
+      </c>
+      <c r="D9" s="20"/>
+      <c r="E9" s="21" t="s">
+        <v>575</v>
+      </c>
+      <c r="F9" s="20"/>
+    </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
     </row>
@@ -2588,18 +2621,19 @@
   <autoFilter ref="B1:B7"/>
   <hyperlinks>
     <hyperlink ref="F8" r:id="rId1"/>
+    <hyperlink ref="E9" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2784,6 +2818,17 @@
         <v>571</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
+        <v>573</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>472</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>574</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2795,7 +2840,7 @@
   <dimension ref="A1:G887"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="A209" sqref="A209:A872"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7595,7 +7640,7 @@
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>472</v>
+        <v>572</v>
       </c>
       <c r="B209" t="s">
         <v>473</v>
@@ -12747,7 +12792,7 @@
     </row>
     <row r="433" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>472</v>
+        <v>572</v>
       </c>
       <c r="B433" t="s">
         <v>473</v>
@@ -17830,7 +17875,7 @@
     </row>
     <row r="654" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A654" t="s">
-        <v>472</v>
+        <v>572</v>
       </c>
       <c r="B654" t="s">
         <v>473</v>
@@ -22844,7 +22889,7 @@
     </row>
     <row r="872" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A872" t="s">
-        <v>472</v>
+        <v>572</v>
       </c>
       <c r="B872" t="s">
         <v>473</v>

</xml_diff>

<commit_message>
fix bugs in wdc-i18n
</commit_message>
<xml_diff>
--- a/wdc_libs/data-examples/dataset-example.xlsx
+++ b/wdc_libs/data-examples/dataset-example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="15120" windowHeight="7830" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="15120" windowHeight="7830"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="5" r:id="rId1"/>
@@ -1556,9 +1556,6 @@
     <t>dataset.commit.note</t>
   </si>
   <si>
-    <t>Add commit info</t>
-  </si>
-  <si>
     <t>#GDP</t>
   </si>
   <si>
@@ -1748,7 +1745,10 @@
     <t>Україна</t>
   </si>
   <si>
-    <t>https://flagspot.net/images/u/ua.gif</t>
+    <t>http://flags.fmcdn.net/data/flags/mini/ua.png</t>
+  </si>
+  <si>
+    <t>Add UA flag</t>
   </si>
 </sst>
 </file>
@@ -2224,8 +2224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2248,15 +2248,15 @@
         <v>22</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2269,10 +2269,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2280,24 +2280,24 @@
         <v>510</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>511</v>
+        <v>575</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B7" s="13">
         <f ca="1">TODAY()</f>
-        <v>42346</v>
+        <v>42347</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2310,18 +2310,18 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2337,15 +2337,15 @@
         <v>35</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2358,10 +2358,10 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2374,10 +2374,10 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2461,8 +2461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2481,19 +2481,19 @@
         <v>11</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>538</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>539</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>540</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -2504,10 +2504,10 @@
         <v>23</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>30</v>
@@ -2518,52 +2518,52 @@
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>46</v>
@@ -2574,7 +2574,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>46</v>
@@ -2585,32 +2585,32 @@
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
+        <v>562</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>563</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="5" t="s">
+        <v>565</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>564</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="F8" s="17" t="s">
         <v>566</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>565</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B9" s="19"/>
       <c r="C9" s="20" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D9" s="20"/>
       <c r="E9" s="21" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F9" s="20"/>
     </row>
@@ -2647,26 +2647,26 @@
         <v>11</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>541</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>542</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>6</v>
@@ -2677,7 +2677,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>18</v>
@@ -2688,18 +2688,18 @@
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>31</v>
@@ -2710,29 +2710,29 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>524</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>525</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>14</v>
@@ -2743,7 +2743,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>15</v>
@@ -2754,7 +2754,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>9</v>
@@ -2765,68 +2765,68 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
+        <v>547</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>548</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="C12" s="15" t="s">
         <v>549</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
+        <v>551</v>
+      </c>
+      <c r="B13" s="15" t="s">
         <v>552</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="C13" s="15" t="s">
         <v>553</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
+        <v>556</v>
+      </c>
+      <c r="B14" t="s">
+        <v>558</v>
+      </c>
+      <c r="C14" s="16" t="s">
         <v>557</v>
-      </c>
-      <c r="B14" t="s">
-        <v>559</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B17" s="20" t="s">
         <v>472</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
   </sheetData>
@@ -7640,7 +7640,7 @@
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B209" t="s">
         <v>473</v>
@@ -12792,7 +12792,7 @@
     </row>
     <row r="433" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B433" t="s">
         <v>473</v>
@@ -17875,7 +17875,7 @@
     </row>
     <row r="654" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A654" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B654" t="s">
         <v>473</v>
@@ -22889,7 +22889,7 @@
     </row>
     <row r="872" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A872" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B872" t="s">
         <v>473</v>

</xml_diff>